<commit_message>
getriebe Umsetzung und Lager CAD60000
</commit_message>
<xml_diff>
--- a/0_Projektorga/RoadMap.xlsx
+++ b/0_Projektorga/RoadMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janbantle/Documents/GitHub/Studienarbeit/0_Projektorga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F34151-F7EA-4E4D-B634-DF2BB6AD71E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE05C4E-23B4-464A-B932-DDD592868C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{FA9784DD-23F6-4C9A-9C04-5F94D8053CAD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
   <si>
     <t xml:space="preserve">Oktober </t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Fertigung Riemenrad I</t>
+  </si>
+  <si>
+    <t>Anforderungsanalyse Mechanik</t>
   </si>
 </sst>
 </file>
@@ -1179,45 +1182,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1263,16 +1227,55 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3780,24 +3783,24 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16">
       <c r="A1" s="23"/>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="82" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="85" t="s">
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="86"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="73"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15">
@@ -3902,26 +3905,26 @@
       <c r="A5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="78" t="s">
+      <c r="C5" s="92"/>
+      <c r="D5" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="81"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="74" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="12"/>
@@ -3939,7 +3942,7 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A7" s="88"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="12"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3955,7 +3958,7 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A8" s="89"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="12"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -3971,7 +3974,7 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="77" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="13"/>
@@ -3989,7 +3992,7 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A10" s="91"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="13"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4005,7 +4008,7 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A11" s="92"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="13"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -4021,7 +4024,7 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="85" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="14"/>
@@ -4039,7 +4042,7 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A13" s="71"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="14"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -4055,7 +4058,7 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A14" s="72"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="14"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -4071,7 +4074,7 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="88" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="5"/>
@@ -4089,7 +4092,7 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A16" s="74"/>
+      <c r="A16" s="89"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -4105,7 +4108,7 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="16" thickBot="1">
-      <c r="A17" s="75"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -4121,7 +4124,7 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="82" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="32"/>
@@ -4138,7 +4141,7 @@
       <c r="M18" s="34"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="68"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -4153,7 +4156,7 @@
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="1:14" ht="15" thickBot="1">
-      <c r="A20" s="69"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
@@ -4169,17 +4172,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:K5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:K5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B6:J14">
@@ -4246,11 +4249,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08215EA3-8C9C-604B-8B92-D34B0C342221}">
-  <dimension ref="A1:HM37"/>
+  <dimension ref="A1:HM38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
+      <selection pane="topRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="14"/>
@@ -4282,357 +4285,357 @@
   <sheetData>
     <row r="1" spans="1:221" s="41" customFormat="1">
       <c r="A1" s="38"/>
-      <c r="B1" s="98">
+      <c r="B1" s="95">
         <v>44473</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98">
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95">
         <f>B1+7</f>
         <v>44480</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98">
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95">
         <f t="shared" ref="L1" si="0">G1+7</f>
         <v>44487</v>
       </c>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98">
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95">
         <f t="shared" ref="Q1" si="1">L1+7</f>
         <v>44494</v>
       </c>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98">
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95">
         <f t="shared" ref="V1" si="2">Q1+7</f>
         <v>44501</v>
       </c>
-      <c r="W1" s="98"/>
-      <c r="X1" s="98"/>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="98"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
       <c r="AA1" s="99">
         <f t="shared" ref="AA1" si="3">V1+7</f>
         <v>44508</v>
       </c>
-      <c r="AB1" s="98"/>
-      <c r="AC1" s="98"/>
-      <c r="AD1" s="98"/>
+      <c r="AB1" s="95"/>
+      <c r="AC1" s="95"/>
+      <c r="AD1" s="95"/>
       <c r="AE1" s="100"/>
       <c r="AF1" s="99">
         <f t="shared" ref="AF1" si="4">AA1+7</f>
         <v>44515</v>
       </c>
-      <c r="AG1" s="98"/>
-      <c r="AH1" s="98"/>
-      <c r="AI1" s="98"/>
+      <c r="AG1" s="95"/>
+      <c r="AH1" s="95"/>
+      <c r="AI1" s="95"/>
       <c r="AJ1" s="100"/>
       <c r="AK1" s="99">
         <f t="shared" ref="AK1" si="5">AF1+7</f>
         <v>44522</v>
       </c>
-      <c r="AL1" s="98"/>
-      <c r="AM1" s="98"/>
-      <c r="AN1" s="98"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
       <c r="AO1" s="100"/>
       <c r="AP1" s="99">
         <f t="shared" ref="AP1" si="6">AK1+7</f>
         <v>44529</v>
       </c>
-      <c r="AQ1" s="98"/>
-      <c r="AR1" s="98"/>
-      <c r="AS1" s="98"/>
+      <c r="AQ1" s="95"/>
+      <c r="AR1" s="95"/>
+      <c r="AS1" s="95"/>
       <c r="AT1" s="100"/>
       <c r="AU1" s="99">
         <f t="shared" ref="AU1" si="7">AP1+7</f>
         <v>44536</v>
       </c>
-      <c r="AV1" s="98"/>
-      <c r="AW1" s="98"/>
-      <c r="AX1" s="98"/>
+      <c r="AV1" s="95"/>
+      <c r="AW1" s="95"/>
+      <c r="AX1" s="95"/>
       <c r="AY1" s="100"/>
       <c r="AZ1" s="99">
         <f t="shared" ref="AZ1" si="8">AU1+7</f>
         <v>44543</v>
       </c>
-      <c r="BA1" s="98"/>
-      <c r="BB1" s="98"/>
-      <c r="BC1" s="98"/>
+      <c r="BA1" s="95"/>
+      <c r="BB1" s="95"/>
+      <c r="BC1" s="95"/>
       <c r="BD1" s="100"/>
       <c r="BE1" s="99">
         <f t="shared" ref="BE1" si="9">AZ1+7</f>
         <v>44550</v>
       </c>
-      <c r="BF1" s="98"/>
-      <c r="BG1" s="98"/>
-      <c r="BH1" s="98"/>
+      <c r="BF1" s="95"/>
+      <c r="BG1" s="95"/>
+      <c r="BH1" s="95"/>
       <c r="BI1" s="100"/>
-      <c r="BJ1" s="98">
+      <c r="BJ1" s="95">
         <f t="shared" ref="BJ1" si="10">BE1+7</f>
         <v>44557</v>
       </c>
-      <c r="BK1" s="98"/>
-      <c r="BL1" s="98"/>
-      <c r="BM1" s="98"/>
-      <c r="BN1" s="98"/>
-      <c r="BO1" s="98">
+      <c r="BK1" s="95"/>
+      <c r="BL1" s="95"/>
+      <c r="BM1" s="95"/>
+      <c r="BN1" s="95"/>
+      <c r="BO1" s="95">
         <f t="shared" ref="BO1" si="11">BJ1+7</f>
         <v>44564</v>
       </c>
-      <c r="BP1" s="98"/>
-      <c r="BQ1" s="98"/>
-      <c r="BR1" s="98"/>
-      <c r="BS1" s="98"/>
-      <c r="BT1" s="98">
+      <c r="BP1" s="95"/>
+      <c r="BQ1" s="95"/>
+      <c r="BR1" s="95"/>
+      <c r="BS1" s="95"/>
+      <c r="BT1" s="95">
         <f t="shared" ref="BT1" si="12">BO1+7</f>
         <v>44571</v>
       </c>
-      <c r="BU1" s="98"/>
-      <c r="BV1" s="98"/>
-      <c r="BW1" s="98"/>
-      <c r="BX1" s="98"/>
-      <c r="BY1" s="98">
+      <c r="BU1" s="95"/>
+      <c r="BV1" s="95"/>
+      <c r="BW1" s="95"/>
+      <c r="BX1" s="95"/>
+      <c r="BY1" s="95">
         <f t="shared" ref="BY1" si="13">BT1+7</f>
         <v>44578</v>
       </c>
-      <c r="BZ1" s="98"/>
-      <c r="CA1" s="98"/>
-      <c r="CB1" s="98"/>
-      <c r="CC1" s="98"/>
-      <c r="CD1" s="98">
+      <c r="BZ1" s="95"/>
+      <c r="CA1" s="95"/>
+      <c r="CB1" s="95"/>
+      <c r="CC1" s="95"/>
+      <c r="CD1" s="95">
         <f t="shared" ref="CD1" si="14">BY1+7</f>
         <v>44585</v>
       </c>
-      <c r="CE1" s="98"/>
-      <c r="CF1" s="98"/>
-      <c r="CG1" s="98"/>
-      <c r="CH1" s="98"/>
-      <c r="CI1" s="98">
+      <c r="CE1" s="95"/>
+      <c r="CF1" s="95"/>
+      <c r="CG1" s="95"/>
+      <c r="CH1" s="95"/>
+      <c r="CI1" s="95">
         <f t="shared" ref="CI1" si="15">CD1+7</f>
         <v>44592</v>
       </c>
-      <c r="CJ1" s="98"/>
-      <c r="CK1" s="98"/>
-      <c r="CL1" s="98"/>
-      <c r="CM1" s="98"/>
-      <c r="CN1" s="98">
+      <c r="CJ1" s="95"/>
+      <c r="CK1" s="95"/>
+      <c r="CL1" s="95"/>
+      <c r="CM1" s="95"/>
+      <c r="CN1" s="95">
         <f t="shared" ref="CN1" si="16">CI1+7</f>
         <v>44599</v>
       </c>
-      <c r="CO1" s="98"/>
-      <c r="CP1" s="98"/>
-      <c r="CQ1" s="98"/>
-      <c r="CR1" s="98"/>
-      <c r="CS1" s="98">
+      <c r="CO1" s="95"/>
+      <c r="CP1" s="95"/>
+      <c r="CQ1" s="95"/>
+      <c r="CR1" s="95"/>
+      <c r="CS1" s="95">
         <f t="shared" ref="CS1" si="17">CN1+7</f>
         <v>44606</v>
       </c>
-      <c r="CT1" s="98"/>
-      <c r="CU1" s="98"/>
-      <c r="CV1" s="98"/>
-      <c r="CW1" s="98"/>
-      <c r="CX1" s="98">
+      <c r="CT1" s="95"/>
+      <c r="CU1" s="95"/>
+      <c r="CV1" s="95"/>
+      <c r="CW1" s="95"/>
+      <c r="CX1" s="95">
         <f t="shared" ref="CX1" si="18">CS1+7</f>
         <v>44613</v>
       </c>
-      <c r="CY1" s="98"/>
-      <c r="CZ1" s="98"/>
-      <c r="DA1" s="98"/>
-      <c r="DB1" s="98"/>
-      <c r="DC1" s="98">
+      <c r="CY1" s="95"/>
+      <c r="CZ1" s="95"/>
+      <c r="DA1" s="95"/>
+      <c r="DB1" s="95"/>
+      <c r="DC1" s="95">
         <f t="shared" ref="DC1" si="19">CX1+7</f>
         <v>44620</v>
       </c>
-      <c r="DD1" s="98"/>
-      <c r="DE1" s="98"/>
-      <c r="DF1" s="98"/>
-      <c r="DG1" s="98"/>
-      <c r="DH1" s="98">
+      <c r="DD1" s="95"/>
+      <c r="DE1" s="95"/>
+      <c r="DF1" s="95"/>
+      <c r="DG1" s="95"/>
+      <c r="DH1" s="95">
         <f t="shared" ref="DH1" si="20">DC1+7</f>
         <v>44627</v>
       </c>
-      <c r="DI1" s="98"/>
-      <c r="DJ1" s="98"/>
-      <c r="DK1" s="98"/>
-      <c r="DL1" s="98"/>
-      <c r="DM1" s="98">
+      <c r="DI1" s="95"/>
+      <c r="DJ1" s="95"/>
+      <c r="DK1" s="95"/>
+      <c r="DL1" s="95"/>
+      <c r="DM1" s="95">
         <f t="shared" ref="DM1" si="21">DH1+7</f>
         <v>44634</v>
       </c>
-      <c r="DN1" s="98"/>
-      <c r="DO1" s="98"/>
-      <c r="DP1" s="98"/>
-      <c r="DQ1" s="98"/>
-      <c r="DR1" s="98">
+      <c r="DN1" s="95"/>
+      <c r="DO1" s="95"/>
+      <c r="DP1" s="95"/>
+      <c r="DQ1" s="95"/>
+      <c r="DR1" s="95">
         <f t="shared" ref="DR1" si="22">DM1+7</f>
         <v>44641</v>
       </c>
-      <c r="DS1" s="98"/>
-      <c r="DT1" s="98"/>
-      <c r="DU1" s="98"/>
-      <c r="DV1" s="98"/>
-      <c r="DW1" s="98">
+      <c r="DS1" s="95"/>
+      <c r="DT1" s="95"/>
+      <c r="DU1" s="95"/>
+      <c r="DV1" s="95"/>
+      <c r="DW1" s="95">
         <f t="shared" ref="DW1" si="23">DR1+7</f>
         <v>44648</v>
       </c>
-      <c r="DX1" s="98"/>
-      <c r="DY1" s="98"/>
-      <c r="DZ1" s="98"/>
-      <c r="EA1" s="98"/>
-      <c r="EB1" s="98">
+      <c r="DX1" s="95"/>
+      <c r="DY1" s="95"/>
+      <c r="DZ1" s="95"/>
+      <c r="EA1" s="95"/>
+      <c r="EB1" s="95">
         <f t="shared" ref="EB1" si="24">DW1+7</f>
         <v>44655</v>
       </c>
-      <c r="EC1" s="98"/>
-      <c r="ED1" s="98"/>
-      <c r="EE1" s="98"/>
-      <c r="EF1" s="98"/>
-      <c r="EG1" s="98">
+      <c r="EC1" s="95"/>
+      <c r="ED1" s="95"/>
+      <c r="EE1" s="95"/>
+      <c r="EF1" s="95"/>
+      <c r="EG1" s="95">
         <f t="shared" ref="EG1" si="25">EB1+7</f>
         <v>44662</v>
       </c>
-      <c r="EH1" s="98"/>
-      <c r="EI1" s="98"/>
-      <c r="EJ1" s="98"/>
-      <c r="EK1" s="98"/>
-      <c r="EL1" s="98">
+      <c r="EH1" s="95"/>
+      <c r="EI1" s="95"/>
+      <c r="EJ1" s="95"/>
+      <c r="EK1" s="95"/>
+      <c r="EL1" s="95">
         <f t="shared" ref="EL1" si="26">EG1+7</f>
         <v>44669</v>
       </c>
-      <c r="EM1" s="98"/>
-      <c r="EN1" s="98"/>
-      <c r="EO1" s="98"/>
-      <c r="EP1" s="98"/>
-      <c r="EQ1" s="98">
+      <c r="EM1" s="95"/>
+      <c r="EN1" s="95"/>
+      <c r="EO1" s="95"/>
+      <c r="EP1" s="95"/>
+      <c r="EQ1" s="95">
         <f t="shared" ref="EQ1" si="27">EL1+7</f>
         <v>44676</v>
       </c>
-      <c r="ER1" s="98"/>
-      <c r="ES1" s="98"/>
-      <c r="ET1" s="98"/>
-      <c r="EU1" s="98"/>
-      <c r="EV1" s="98">
+      <c r="ER1" s="95"/>
+      <c r="ES1" s="95"/>
+      <c r="ET1" s="95"/>
+      <c r="EU1" s="95"/>
+      <c r="EV1" s="95">
         <f t="shared" ref="EV1" si="28">EQ1+7</f>
         <v>44683</v>
       </c>
-      <c r="EW1" s="98"/>
-      <c r="EX1" s="98"/>
-      <c r="EY1" s="98"/>
-      <c r="EZ1" s="98"/>
-      <c r="FA1" s="98">
+      <c r="EW1" s="95"/>
+      <c r="EX1" s="95"/>
+      <c r="EY1" s="95"/>
+      <c r="EZ1" s="95"/>
+      <c r="FA1" s="95">
         <f t="shared" ref="FA1" si="29">EV1+7</f>
         <v>44690</v>
       </c>
-      <c r="FB1" s="98"/>
-      <c r="FC1" s="98"/>
-      <c r="FD1" s="98"/>
-      <c r="FE1" s="98"/>
-      <c r="FF1" s="98">
+      <c r="FB1" s="95"/>
+      <c r="FC1" s="95"/>
+      <c r="FD1" s="95"/>
+      <c r="FE1" s="95"/>
+      <c r="FF1" s="95">
         <f t="shared" ref="FF1" si="30">FA1+7</f>
         <v>44697</v>
       </c>
-      <c r="FG1" s="98"/>
-      <c r="FH1" s="98"/>
-      <c r="FI1" s="98"/>
-      <c r="FJ1" s="98"/>
-      <c r="FK1" s="98">
+      <c r="FG1" s="95"/>
+      <c r="FH1" s="95"/>
+      <c r="FI1" s="95"/>
+      <c r="FJ1" s="95"/>
+      <c r="FK1" s="95">
         <f t="shared" ref="FK1" si="31">FF1+7</f>
         <v>44704</v>
       </c>
-      <c r="FL1" s="98"/>
-      <c r="FM1" s="98"/>
-      <c r="FN1" s="98"/>
-      <c r="FO1" s="98"/>
-      <c r="FP1" s="98">
+      <c r="FL1" s="95"/>
+      <c r="FM1" s="95"/>
+      <c r="FN1" s="95"/>
+      <c r="FO1" s="95"/>
+      <c r="FP1" s="95">
         <f t="shared" ref="FP1" si="32">FK1+7</f>
         <v>44711</v>
       </c>
-      <c r="FQ1" s="98"/>
-      <c r="FR1" s="98"/>
-      <c r="FS1" s="98"/>
-      <c r="FT1" s="98"/>
-      <c r="FU1" s="98">
+      <c r="FQ1" s="95"/>
+      <c r="FR1" s="95"/>
+      <c r="FS1" s="95"/>
+      <c r="FT1" s="95"/>
+      <c r="FU1" s="95">
         <f t="shared" ref="FU1" si="33">FP1+7</f>
         <v>44718</v>
       </c>
-      <c r="FV1" s="98"/>
-      <c r="FW1" s="98"/>
-      <c r="FX1" s="98"/>
-      <c r="FY1" s="98"/>
-      <c r="FZ1" s="98">
+      <c r="FV1" s="95"/>
+      <c r="FW1" s="95"/>
+      <c r="FX1" s="95"/>
+      <c r="FY1" s="95"/>
+      <c r="FZ1" s="95">
         <f t="shared" ref="FZ1" si="34">FU1+7</f>
         <v>44725</v>
       </c>
-      <c r="GA1" s="98"/>
-      <c r="GB1" s="98"/>
-      <c r="GC1" s="98"/>
-      <c r="GD1" s="98"/>
-      <c r="GE1" s="98">
+      <c r="GA1" s="95"/>
+      <c r="GB1" s="95"/>
+      <c r="GC1" s="95"/>
+      <c r="GD1" s="95"/>
+      <c r="GE1" s="95">
         <f t="shared" ref="GE1" si="35">FZ1+7</f>
         <v>44732</v>
       </c>
-      <c r="GF1" s="98"/>
-      <c r="GG1" s="98"/>
-      <c r="GH1" s="98"/>
-      <c r="GI1" s="98"/>
-      <c r="GJ1" s="98">
+      <c r="GF1" s="95"/>
+      <c r="GG1" s="95"/>
+      <c r="GH1" s="95"/>
+      <c r="GI1" s="95"/>
+      <c r="GJ1" s="95">
         <f t="shared" ref="GJ1" si="36">GE1+7</f>
         <v>44739</v>
       </c>
-      <c r="GK1" s="98"/>
-      <c r="GL1" s="98"/>
-      <c r="GM1" s="98"/>
-      <c r="GN1" s="98"/>
-      <c r="GO1" s="98">
+      <c r="GK1" s="95"/>
+      <c r="GL1" s="95"/>
+      <c r="GM1" s="95"/>
+      <c r="GN1" s="95"/>
+      <c r="GO1" s="95">
         <f t="shared" ref="GO1" si="37">GJ1+7</f>
         <v>44746</v>
       </c>
-      <c r="GP1" s="98"/>
-      <c r="GQ1" s="98"/>
-      <c r="GR1" s="98"/>
-      <c r="GS1" s="98"/>
-      <c r="GT1" s="98">
+      <c r="GP1" s="95"/>
+      <c r="GQ1" s="95"/>
+      <c r="GR1" s="95"/>
+      <c r="GS1" s="95"/>
+      <c r="GT1" s="95">
         <f t="shared" ref="GT1" si="38">GO1+7</f>
         <v>44753</v>
       </c>
-      <c r="GU1" s="98"/>
-      <c r="GV1" s="98"/>
-      <c r="GW1" s="98"/>
-      <c r="GX1" s="98"/>
-      <c r="GY1" s="98">
+      <c r="GU1" s="95"/>
+      <c r="GV1" s="95"/>
+      <c r="GW1" s="95"/>
+      <c r="GX1" s="95"/>
+      <c r="GY1" s="95">
         <f t="shared" ref="GY1" si="39">GT1+7</f>
         <v>44760</v>
       </c>
-      <c r="GZ1" s="98"/>
-      <c r="HA1" s="98"/>
-      <c r="HB1" s="98"/>
-      <c r="HC1" s="98"/>
-      <c r="HD1" s="98">
+      <c r="GZ1" s="95"/>
+      <c r="HA1" s="95"/>
+      <c r="HB1" s="95"/>
+      <c r="HC1" s="95"/>
+      <c r="HD1" s="95">
         <f t="shared" ref="HD1" si="40">GY1+7</f>
         <v>44767</v>
       </c>
-      <c r="HE1" s="98"/>
-      <c r="HF1" s="98"/>
-      <c r="HG1" s="98"/>
-      <c r="HH1" s="98"/>
-      <c r="HI1" s="98">
+      <c r="HE1" s="95"/>
+      <c r="HF1" s="95"/>
+      <c r="HG1" s="95"/>
+      <c r="HH1" s="95"/>
+      <c r="HI1" s="95">
         <f t="shared" ref="HI1" si="41">HD1+7</f>
         <v>44774</v>
       </c>
-      <c r="HJ1" s="98"/>
-      <c r="HK1" s="98"/>
-      <c r="HL1" s="98"/>
-      <c r="HM1" s="98"/>
+      <c r="HJ1" s="95"/>
+      <c r="HK1" s="95"/>
+      <c r="HL1" s="95"/>
+      <c r="HM1" s="95"/>
     </row>
     <row r="2" spans="1:221" s="43" customFormat="1" ht="15" thickBot="1">
       <c r="A2" s="42"/>
@@ -4671,55 +4674,55 @@
       <c r="X2" s="96"/>
       <c r="Y2" s="96"/>
       <c r="Z2" s="96"/>
-      <c r="AA2" s="95" t="s">
+      <c r="AA2" s="97" t="s">
         <v>4</v>
       </c>
       <c r="AB2" s="96"/>
       <c r="AC2" s="96"/>
       <c r="AD2" s="96"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="95" t="s">
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="97" t="s">
         <v>5</v>
       </c>
       <c r="AG2" s="96"/>
       <c r="AH2" s="96"/>
       <c r="AI2" s="96"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="95" t="s">
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="97" t="s">
         <v>6</v>
       </c>
       <c r="AL2" s="96"/>
       <c r="AM2" s="96"/>
       <c r="AN2" s="96"/>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="95" t="s">
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="97" t="s">
         <v>7</v>
       </c>
       <c r="AQ2" s="96"/>
       <c r="AR2" s="96"/>
       <c r="AS2" s="96"/>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="95" t="s">
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="97" t="s">
         <v>8</v>
       </c>
       <c r="AV2" s="96"/>
       <c r="AW2" s="96"/>
       <c r="AX2" s="96"/>
-      <c r="AY2" s="97"/>
-      <c r="AZ2" s="95" t="s">
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="97" t="s">
         <v>9</v>
       </c>
       <c r="BA2" s="96"/>
       <c r="BB2" s="96"/>
       <c r="BC2" s="96"/>
-      <c r="BD2" s="97"/>
-      <c r="BE2" s="95" t="s">
+      <c r="BD2" s="98"/>
+      <c r="BE2" s="97" t="s">
         <v>10</v>
       </c>
       <c r="BF2" s="96"/>
       <c r="BG2" s="96"/>
       <c r="BH2" s="96"/>
-      <c r="BI2" s="97"/>
+      <c r="BI2" s="98"/>
       <c r="BJ2" s="96" t="s">
         <v>54</v>
       </c>
@@ -10720,31 +10723,67 @@
       <c r="GK37" s="60"/>
       <c r="GL37" s="60"/>
     </row>
+    <row r="38" spans="1:194">
+      <c r="A38" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK38" s="64"/>
+      <c r="AL38" s="64"/>
+      <c r="AM38" s="64"/>
+      <c r="AN38" s="64"/>
+      <c r="AO38" s="64"/>
+    </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="GY1:HC1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="GY2:HC2"/>
-    <mergeCell ref="HD2:HH2"/>
-    <mergeCell ref="HI2:HM2"/>
-    <mergeCell ref="GT2:GX2"/>
-    <mergeCell ref="EQ2:EU2"/>
-    <mergeCell ref="EV2:EZ2"/>
-    <mergeCell ref="FA2:FE2"/>
-    <mergeCell ref="FF2:FJ2"/>
-    <mergeCell ref="FK2:FO2"/>
-    <mergeCell ref="FP2:FT2"/>
-    <mergeCell ref="FU2:FY2"/>
-    <mergeCell ref="FZ2:GD2"/>
-    <mergeCell ref="GE2:GI2"/>
-    <mergeCell ref="GJ2:GN2"/>
-    <mergeCell ref="GO2:GS2"/>
-    <mergeCell ref="DM2:DQ2"/>
-    <mergeCell ref="DR2:DV2"/>
-    <mergeCell ref="DW2:EA2"/>
-    <mergeCell ref="EB2:EF2"/>
-    <mergeCell ref="EG2:EK2"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="AP2:AT2"/>
+    <mergeCell ref="AU2:AY2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BT1:BX1"/>
+    <mergeCell ref="AZ2:BD2"/>
+    <mergeCell ref="BE2:BI2"/>
+    <mergeCell ref="BJ2:BN2"/>
+    <mergeCell ref="BO2:BS2"/>
+    <mergeCell ref="BT2:BX2"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="EB1:EF1"/>
+    <mergeCell ref="BY1:CC1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CI1:CM1"/>
+    <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DH1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="DR1:DV1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="GJ1:GN1"/>
+    <mergeCell ref="EG1:EK1"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="EQ1:EU1"/>
+    <mergeCell ref="EV1:EZ1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FF1:FJ1"/>
     <mergeCell ref="EL2:EP2"/>
     <mergeCell ref="GO1:GS1"/>
     <mergeCell ref="GT1:GX1"/>
@@ -10761,55 +10800,29 @@
     <mergeCell ref="FU1:FY1"/>
     <mergeCell ref="FZ1:GD1"/>
     <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GJ1:GN1"/>
-    <mergeCell ref="EG1:EK1"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="EQ1:EU1"/>
-    <mergeCell ref="EV1:EZ1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FF1:FJ1"/>
-    <mergeCell ref="EB1:EF1"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="DR1:DV1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BX1"/>
-    <mergeCell ref="AZ2:BD2"/>
-    <mergeCell ref="BE2:BI2"/>
-    <mergeCell ref="BJ2:BN2"/>
-    <mergeCell ref="BO2:BS2"/>
-    <mergeCell ref="BT2:BX2"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="AP2:AT2"/>
-    <mergeCell ref="AU2:AY2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="DM2:DQ2"/>
+    <mergeCell ref="DR2:DV2"/>
+    <mergeCell ref="DW2:EA2"/>
+    <mergeCell ref="EB2:EF2"/>
+    <mergeCell ref="EG2:EK2"/>
+    <mergeCell ref="GT2:GX2"/>
+    <mergeCell ref="EQ2:EU2"/>
+    <mergeCell ref="EV2:EZ2"/>
+    <mergeCell ref="FA2:FE2"/>
+    <mergeCell ref="FF2:FJ2"/>
+    <mergeCell ref="FK2:FO2"/>
+    <mergeCell ref="FP2:FT2"/>
+    <mergeCell ref="FU2:FY2"/>
+    <mergeCell ref="FZ2:GD2"/>
+    <mergeCell ref="GE2:GI2"/>
+    <mergeCell ref="GJ2:GN2"/>
+    <mergeCell ref="GO2:GS2"/>
+    <mergeCell ref="GY1:HC1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="GY2:HC2"/>
+    <mergeCell ref="HD2:HH2"/>
+    <mergeCell ref="HI2:HM2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>